<commit_message>
final touches before uploading
</commit_message>
<xml_diff>
--- a/assignements/prijs raming.xlsx
+++ b/assignements/prijs raming.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git\Practice-Enterprise-2\assignements\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\dev\workspaces\git\Practice-Enterprise-2\assignements\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BBECD45A-C9E6-4A02-96D2-DEEB6B4E454F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{009DCFAA-EC20-4EB9-8A12-9CA38752198C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7320" yWindow="0" windowWidth="21600" windowHeight="11235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Tabelle1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>component</t>
   </si>
@@ -71,10 +71,28 @@
     <t>PCB</t>
   </si>
   <si>
-    <t>schatting (was 11,8 vorige eer voor mij)</t>
-  </si>
-  <si>
     <t>Samtec FTSH-107-01-L-DV-K-A</t>
+  </si>
+  <si>
+    <t>RP115H331D-T1-FE voltage regulator</t>
+  </si>
+  <si>
+    <t>voor 2:</t>
+  </si>
+  <si>
+    <t>schatting (was 11,8 vorige keer voor mij)</t>
+  </si>
+  <si>
+    <t>5V 1A adapter</t>
+  </si>
+  <si>
+    <t>FTSH-107-01-L-DV-K-A-P-TR stlink header</t>
+  </si>
+  <si>
+    <t>caps/res</t>
+  </si>
+  <si>
+    <t>schatting</t>
   </si>
 </sst>
 </file>
@@ -82,7 +100,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="167" formatCode="#,##0.00\ &quot;€&quot;"/>
+    <numFmt numFmtId="164" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -93,21 +111,28 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="9"/>
+      <sz val="11"/>
       <color rgb="FF0C0D0E"/>
-      <name val="Segoe UI"/>
+      <name val="Calibri"/>
       <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -115,14 +140,146 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -403,205 +560,334 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C3:G19"/>
+  <dimension ref="C2:J20"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J15" sqref="J15"/>
+      <selection activeCell="N9" sqref="N9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="38.5546875" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" customWidth="1"/>
+    <col min="3" max="3" width="38.5703125" customWidth="1"/>
+    <col min="5" max="5" width="11.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C3" t="s">
+    <row r="2" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="3" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" t="s">
+      <c r="D3" s="16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="F3" t="s">
+      <c r="F3" s="16" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C4" t="s">
+      <c r="G3" s="16"/>
+      <c r="H3" s="16"/>
+      <c r="I3" s="16"/>
+      <c r="J3" s="17"/>
+    </row>
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D4">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1">
+      <c r="D4" s="2">
+        <v>1</v>
+      </c>
+      <c r="E4" s="3">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F4" s="1">
+      <c r="F4" s="3">
         <f>D4*E4</f>
         <v>2.2000000000000002</v>
       </c>
-    </row>
-    <row r="5" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C5" t="s">
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
+      <c r="I4" s="2"/>
+      <c r="J4" s="4"/>
+    </row>
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="D5">
-        <v>1</v>
-      </c>
-      <c r="E5" s="1">
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
+      <c r="E5" s="3">
         <v>5.07</v>
       </c>
-      <c r="F5" s="1">
+      <c r="F5" s="3">
         <f t="shared" ref="F5:F18" si="0">D5*E5</f>
         <v>5.07</v>
       </c>
-    </row>
-    <row r="6" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C6" t="s">
+      <c r="G5" s="2"/>
+      <c r="H5" s="2"/>
+      <c r="I5" s="2"/>
+      <c r="J5" s="4"/>
+    </row>
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6" s="1">
+      <c r="D6" s="2">
+        <v>1</v>
+      </c>
+      <c r="E6" s="3">
         <v>7.96</v>
       </c>
-      <c r="F6" s="1">
+      <c r="F6" s="3">
         <f t="shared" si="0"/>
         <v>7.96</v>
       </c>
-    </row>
-    <row r="7" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C7" t="s">
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="4"/>
+    </row>
+    <row r="7" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="2">
         <v>4</v>
       </c>
-      <c r="E7" s="1">
+      <c r="E7" s="3">
         <v>7.3999999999999996E-2</v>
       </c>
-      <c r="F7" s="1">
+      <c r="F7" s="3">
         <f t="shared" si="0"/>
         <v>0.29599999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C8" t="s">
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+      <c r="J7" s="4"/>
+    </row>
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="D8">
-        <v>1</v>
-      </c>
-      <c r="E8" s="1">
+      <c r="D8" s="2">
+        <v>1</v>
+      </c>
+      <c r="E8" s="3">
         <v>13.1</v>
       </c>
-      <c r="F8" s="1">
+      <c r="F8" s="3">
         <f t="shared" si="0"/>
         <v>13.1</v>
       </c>
-    </row>
-    <row r="9" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C9" t="s">
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+      <c r="J8" s="4"/>
+    </row>
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C9" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D9">
-        <v>1</v>
-      </c>
-      <c r="E9" s="1">
+      <c r="D9" s="2">
+        <v>1</v>
+      </c>
+      <c r="E9" s="3">
         <v>15</v>
       </c>
-      <c r="F9" s="1">
+      <c r="F9" s="3">
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G9" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+      <c r="J9" s="4"/>
+    </row>
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C10" s="5" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="10" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2">
+        <v>1</v>
+      </c>
+      <c r="E10" s="3">
+        <v>5.85</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="0"/>
+        <v>5.85</v>
+      </c>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+      <c r="J10" s="4"/>
+    </row>
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C11" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-      <c r="E10" s="1">
-        <v>5.85</v>
-      </c>
-      <c r="F10" s="1">
-        <f t="shared" si="0"/>
-        <v>5.85</v>
-      </c>
-    </row>
-    <row r="11" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E11" s="1"/>
-      <c r="F11" s="1">
+      <c r="D11" s="2">
+        <v>1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="0"/>
+        <v>1.1200000000000001</v>
+      </c>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+      <c r="J11" s="4"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C12" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="14">
+        <v>1</v>
+      </c>
+      <c r="E12" s="3">
+        <v>6.75</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="0"/>
+        <v>6.75</v>
+      </c>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+      <c r="J12" s="4"/>
+    </row>
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="14">
+        <v>1</v>
+      </c>
+      <c r="E13" s="3">
+        <v>4.03</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="0"/>
+        <v>4.03</v>
+      </c>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+      <c r="J13" s="4"/>
+    </row>
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C14" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="14">
+        <v>1</v>
+      </c>
+      <c r="E14" s="3">
+        <v>5</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+      <c r="J14" s="4"/>
+    </row>
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C15" s="1"/>
+      <c r="D15" s="2"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E12" s="1"/>
-      <c r="F12" s="1">
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+      <c r="J15" s="4"/>
+    </row>
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C16" s="1"/>
+      <c r="D16" s="2"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E13" s="1"/>
-      <c r="F13" s="1">
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+      <c r="J16" s="4"/>
+    </row>
+    <row r="17" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C17" s="1"/>
+      <c r="D17" s="2"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E14" s="1"/>
-      <c r="F14" s="1">
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+      <c r="I17" s="2"/>
+      <c r="J17" s="4"/>
+    </row>
+    <row r="18" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C18" s="10"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E15" s="1"/>
-      <c r="F15" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="3:7" x14ac:dyDescent="0.3">
-      <c r="E16" s="1"/>
-      <c r="F16" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E17" s="1"/>
-      <c r="F17" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="F18" s="1">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="5:6" x14ac:dyDescent="0.3">
-      <c r="E19" t="s">
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="13"/>
+    </row>
+    <row r="19" spans="3:10" x14ac:dyDescent="0.25">
+      <c r="C19" s="1"/>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F19" s="1">
+      <c r="F19" s="3">
         <f>SUM(F4:F18)</f>
-        <v>49.475999999999999</v>
-      </c>
+        <v>66.376000000000005</v>
+      </c>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+      <c r="I19" s="2"/>
+      <c r="J19" s="4"/>
+    </row>
+    <row r="20" spans="3:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="6"/>
+      <c r="D20" s="7"/>
+      <c r="E20" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="F20" s="8">
+        <f>F19*2</f>
+        <v>132.75200000000001</v>
+      </c>
+      <c r="G20" s="7"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>